<commit_message>
Breytti excel, eyddi skritnum .py
</commit_message>
<xml_diff>
--- a/VerkefnataflaBurnDown.xlsx
+++ b/VerkefnataflaBurnDown.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="5715" windowHeight="7740"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="5715" windowHeight="7740" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Notendasögur" sheetId="1" r:id="rId1"/>
-    <sheet name="Burn-Down" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Fallaforritun" sheetId="3" r:id="rId2"/>
+    <sheet name="Burn-Down" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="63">
   <si>
     <t>Textentry</t>
   </si>
@@ -225,6 +225,64 @@
   </si>
   <si>
     <t>Ítrun 2</t>
+  </si>
+  <si>
+    <t>Klasi</t>
+  </si>
+  <si>
+    <t>Lýsing</t>
+  </si>
+  <si>
+    <t>Já</t>
+  </si>
+  <si>
+    <t>AccountType.py</t>
+  </si>
+  <si>
+    <t>Klasi sem heldur utan um mismunandi reikninga sem eru lesnir úr skrá.</t>
+  </si>
+  <si>
+    <t>calcLoanFun.py</t>
+  </si>
+  <si>
+    <t>sem segir til um hvað á eftir að borga af láninu</t>
+  </si>
+  <si>
+    <r>
+      <t>Inniheldur</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Loan</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> sem sér um helstu upplýsingar hvers láns og </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>calcLoan</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -693,11 +751,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="138192768"/>
-        <c:axId val="138194304"/>
+        <c:axId val="119200384"/>
+        <c:axId val="122356096"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="138192768"/>
+        <c:axId val="119200384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -705,13 +763,13 @@
         <c:numFmt formatCode="d/m/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="138194304"/>
+        <c:crossAx val="122356096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="138194304"/>
+        <c:axId val="122356096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -725,7 +783,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="138192768"/>
+        <c:crossAx val="119200384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -776,7 +834,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1061,11 +1119,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="122686080"/>
-        <c:axId val="135541120"/>
+        <c:axId val="122385920"/>
+        <c:axId val="122387456"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="122686080"/>
+        <c:axId val="122385920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1073,13 +1131,13 @@
         <c:numFmt formatCode="d/m/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135541120"/>
+        <c:crossAx val="122387456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="135541120"/>
+        <c:axId val="122387456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1093,7 +1151,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="122686080"/>
+        <c:crossAx val="122385920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1144,7 +1202,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1218,6 +1276,18 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C41" totalsRowShown="0">
+  <autoFilter ref="A1:C41"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Klasi"/>
+    <tableColumn id="2" name="Lýsing"/>
+    <tableColumn id="3" name="Já"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1507,8 +1577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="U25" sqref="T25:U25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2037,10 +2107,65 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="65.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="B4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:Q19"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2252,16 +2377,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>